<commit_message>
all plots have been updated to use the custom style and their save locations checked to be consistent
</commit_message>
<xml_diff>
--- a/reports/experiment_tracking_master.xlsx
+++ b/reports/experiment_tracking_master.xlsx
@@ -557,40 +557,40 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.0138</v>
+        <v>0.0144</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0111</v>
+        <v>0.0102</v>
       </c>
       <c r="J2" t="n">
-        <v>0.995</v>
+        <v>0.994</v>
       </c>
       <c r="K2" t="n">
-        <v>0.008699999999999999</v>
+        <v>0.0055</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9951</v>
+        <v>0.994</v>
       </c>
       <c r="M2" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.0054</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9903</v>
+        <v>0.9902</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0167</v>
+        <v>0.0119</v>
       </c>
       <c r="P2" t="n">
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>0.0045</v>
       </c>
       <c r="R2" t="n">
-        <v>0.995</v>
+        <v>0.994</v>
       </c>
       <c r="S2" t="n">
-        <v>0.008699999999999999</v>
+        <v>0.0055</v>
       </c>
     </row>
     <row r="3">
@@ -620,40 +620,40 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.0152</v>
+        <v>0.0154</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0106</v>
+        <v>0.0094</v>
       </c>
       <c r="J3" t="n">
-        <v>0.995</v>
+        <v>0.9945000000000001</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0067</v>
+        <v>0.005</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9951</v>
+        <v>0.9945000000000001</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0066</v>
+        <v>0.0049</v>
       </c>
       <c r="N3" t="n">
-        <v>0.9903</v>
+        <v>0.9902</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0129</v>
+        <v>0.0103</v>
       </c>
       <c r="P3" t="n">
-        <v>1</v>
+        <v>0.999</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>0.0032</v>
       </c>
       <c r="R3" t="n">
-        <v>0.995</v>
+        <v>0.9945000000000001</v>
       </c>
       <c r="S3" t="n">
-        <v>0.0067</v>
+        <v>0.005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added functionality to generate a standalone training dataset with seed 99. 10 other seeded datasets 0-9 are generated and will be unseen to to the model.
</commit_message>
<xml_diff>
--- a/reports/experiment_tracking_master.xlsx
+++ b/reports/experiment_tracking_master.xlsx
@@ -557,40 +557,40 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.0144</v>
+        <v>0.0155</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0102</v>
+        <v>0.0083</v>
       </c>
       <c r="J2" t="n">
-        <v>0.994</v>
+        <v>0.993</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0055</v>
+        <v>0.0057</v>
       </c>
       <c r="L2" t="n">
-        <v>0.994</v>
+        <v>0.9931</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0054</v>
+        <v>0.0056</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9902</v>
+        <v>0.9863</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0119</v>
+        <v>0.0111</v>
       </c>
       <c r="P2" t="n">
-        <v>0.998</v>
+        <v>1</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0045</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>0.994</v>
+        <v>0.993</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0055</v>
+        <v>0.0057</v>
       </c>
     </row>
     <row r="3">
@@ -620,40 +620,40 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.0154</v>
+        <v>0.0139</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0094</v>
+        <v>0.0071</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9945000000000001</v>
+        <v>0.994</v>
       </c>
       <c r="K3" t="n">
-        <v>0.005</v>
+        <v>0.0046</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9945000000000001</v>
+        <v>0.9941</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0049</v>
+        <v>0.0045</v>
       </c>
       <c r="N3" t="n">
-        <v>0.9902</v>
+        <v>0.9882</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0103</v>
+        <v>0.0089</v>
       </c>
       <c r="P3" t="n">
-        <v>0.999</v>
+        <v>1</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.0032</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.9945000000000001</v>
+        <v>0.994</v>
       </c>
       <c r="S3" t="n">
-        <v>0.005</v>
+        <v>0.0046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generation - comparison pipeline working and plots all in correct locations
</commit_message>
<xml_diff>
--- a/reports/experiment_tracking_master.xlsx
+++ b/reports/experiment_tracking_master.xlsx
@@ -557,40 +557,40 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.0155</v>
+        <v>0.0321</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0083</v>
+        <v>0.0053</v>
       </c>
       <c r="J2" t="n">
-        <v>0.993</v>
+        <v>0.9899</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0057</v>
+        <v>0.0026</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9931</v>
+        <v>0.9899</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0056</v>
+        <v>0.0026</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9863</v>
+        <v>0.9916</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0111</v>
+        <v>0.0028</v>
       </c>
       <c r="P2" t="n">
-        <v>1</v>
+        <v>0.9882</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>0.0048</v>
       </c>
       <c r="R2" t="n">
-        <v>0.993</v>
+        <v>0.9899</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0057</v>
+        <v>0.0026</v>
       </c>
     </row>
     <row r="3">
@@ -620,40 +620,40 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.0139</v>
+        <v>0.0324</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0071</v>
+        <v>0.0052</v>
       </c>
       <c r="J3" t="n">
-        <v>0.994</v>
+        <v>0.9898</v>
       </c>
       <c r="K3" t="n">
+        <v>0.0027</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.9898</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0027</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.9913999999999999</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.0031</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.9882</v>
+      </c>
+      <c r="Q3" t="n">
         <v>0.0046</v>
       </c>
-      <c r="L3" t="n">
-        <v>0.9941</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.0045</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.9882</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.0089</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
       <c r="R3" t="n">
-        <v>0.994</v>
+        <v>0.9898</v>
       </c>
       <c r="S3" t="n">
-        <v>0.0046</v>
+        <v>0.0027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>